<commit_message>
Korrigert farge til Fredlogo på hjemmeside
</commit_message>
<xml_diff>
--- a/åpål/forsendelse_norgespakke.xlsx
+++ b/åpål/forsendelse_norgespakke.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Volum</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>Høyde</t>
+  </si>
+  <si>
+    <t>Mekkeske</t>
   </si>
 </sst>
 </file>
@@ -408,15 +411,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="C5:E5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -433,7 +436,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>C2*D2*E2/100^3</f>
         <v>2.0937999999999998E-2</v>
@@ -451,7 +454,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>B3/B2*A2</f>
         <v>7.851749999999999E-2</v>
@@ -461,7 +464,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>C4*D4*E4/100^3</f>
         <v>0.03</v>
@@ -480,7 +483,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>C5*D5*E5/100^3</f>
         <v>0.432</v>
@@ -499,23 +502,31 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>C7*D7*E7/100^3</f>
-        <v>8.5956000000000005E-2</v>
+        <v>8.1645695999999976E-2</v>
       </c>
       <c r="B7">
         <f>A7/A5*B5</f>
-        <v>32.842105263157904</v>
+        <v>31.195222466329156</v>
       </c>
       <c r="C7">
-        <v>58</v>
+        <v>57.6</v>
       </c>
       <c r="D7">
-        <v>39</v>
+        <v>37.4</v>
       </c>
       <c r="E7">
-        <v>38</v>
+        <v>37.9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>0.37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>